<commit_message>
monthly budget totally integrated
</commit_message>
<xml_diff>
--- a/Test Cases.xlsx
+++ b/Test Cases.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\nisha\Desktop\College Stuff\Internship - 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bhave\Desktop\files\projects\internship-2\ProjectBudgetTracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{786E815F-C3EE-4485-ADA2-37C0703D6D4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CE57DA0-3331-429F-818B-F68B0867ED71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D8F71A25-BE22-496E-83DB-7B3F4B7EA1D2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D8F71A25-BE22-496E-83DB-7B3F4B7EA1D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Project 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -115,7 +115,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="170" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+    <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -214,13 +214,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="170" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -540,20 +540,20 @@
   <dimension ref="C4:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="28.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="19.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="2" width="9.109375" style="1"/>
+    <col min="3" max="3" width="28.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="19.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C4" s="4" t="s">
         <v>12</v>
       </c>
@@ -576,7 +576,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C5" s="5" t="s">
         <v>18</v>
       </c>
@@ -591,7 +591,7 @@
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
     </row>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C6" s="5" t="s">
         <v>6</v>
       </c>
@@ -600,13 +600,13 @@
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="8">
-        <v>200000</v>
+        <v>300000</v>
       </c>
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
     </row>
-    <row r="7" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C7" s="5" t="s">
         <v>7</v>
       </c>
@@ -621,7 +621,7 @@
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
     </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C8" s="5" t="s">
         <v>8</v>
       </c>
@@ -633,13 +633,13 @@
       </c>
       <c r="F8" s="8">
         <f>F6-F7</f>
-        <v>-126000</v>
+        <v>-26000</v>
       </c>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
     </row>
-    <row r="9" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C9" s="5" t="s">
         <v>9</v>
       </c>
@@ -651,13 +651,13 @@
       </c>
       <c r="F9" s="10">
         <f>F6/F7</f>
-        <v>0.61349693251533743</v>
+        <v>0.92024539877300615</v>
       </c>
       <c r="G9" s="10"/>
       <c r="H9" s="10"/>
       <c r="I9" s="10"/>
     </row>
-    <row r="10" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C10" s="5" t="s">
         <v>10</v>
       </c>
@@ -669,13 +669,13 @@
       </c>
       <c r="F10" s="8">
         <f>F5/F9</f>
-        <v>1059500</v>
+        <v>706333.33333333337</v>
       </c>
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
       <c r="I10" s="8"/>
     </row>
-    <row r="11" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C11" s="5" t="s">
         <v>15</v>
       </c>
@@ -687,7 +687,7 @@
       </c>
       <c r="F11" s="8">
         <f>F5-F10</f>
-        <v>-409500</v>
+        <v>-56333.333333333372</v>
       </c>
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>

</xml_diff>